<commit_message>
Add levels 7-1 7-2 8-1 8-2 9-1 9-2
</commit_message>
<xml_diff>
--- a/todo-lvl.xlsx
+++ b/todo-lvl.xlsx
@@ -265,43 +265,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <condense val="0"/>
@@ -631,7 +595,7 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -720,13 +684,13 @@
         <v>6</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="15.75" thickBot="1">
@@ -752,13 +716,13 @@
         <v>6</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -784,13 +748,13 @@
         <v>6</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -816,13 +780,13 @@
         <v>6</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -1157,7 +1121,7 @@
       </c>
       <c r="F18" s="8">
         <f>COUNTIF($B$3:$J$16, "ok")/126</f>
-        <v>0.66666666666666663</v>
+        <v>0.76190476190476186</v>
       </c>
       <c r="G18" s="9"/>
     </row>
@@ -1170,13 +1134,13 @@
     <mergeCell ref="F18:G19"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:E18 G3:G18 F3:F17 H3:J16">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
       <formula>"todo"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"test"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"ok"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>